<commit_message>
started work on standardisation + cleaning up + unit tests
</commit_message>
<xml_diff>
--- a/Excelutilities/weird_to_standard/weird_to_standard1/wts_1_preprocessing_example.xlsx
+++ b/Excelutilities/weird_to_standard/weird_to_standard1/wts_1_preprocessing_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\excel-utilities\Excelutilities\weird_to_standard\weird_to_standard1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D2B00C-CCAA-4658-836F-EC3337506C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC237BF5-ECC2-4E98-9A9A-5C6EB6294E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4635" yWindow="2647" windowWidth="14400" windowHeight="8273" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>